<commit_message>
Removed old data folder, renamed
</commit_message>
<xml_diff>
--- a/Data/WWTP/WWTP_location.xlsx
+++ b/Data/WWTP/WWTP_location.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uthtmc-my.sharepoint.com/personal/hieu_t_nguyen_uth_tmc_edu1/Documents/TEPHI_WW_Dashboard/Data/WWTP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uthtmc-my.sharepoint.com/personal/hieu_t_nguyen_uth_tmc_edu1/Documents/TEPHI_WW_RShinyDashboard/Data/WWTP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="217" documentId="13_ncr:1_{D31C9E89-BFD8-4A4B-8DE6-C69F891C6CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C85A9BD-46E0-2C4A-B70C-00F32D4B373C}"/>
+  <xr:revisionPtr revIDLastSave="219" documentId="13_ncr:1_{D31C9E89-BFD8-4A4B-8DE6-C69F891C6CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7F368DD-B4B1-4A77-9CCF-0DA507DB64DA}"/>
   <bookViews>
-    <workbookView xWindow="8860" yWindow="500" windowWidth="19940" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39825" yWindow="4080" windowWidth="22200" windowHeight="20910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +176,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -201,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -209,6 +216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -226,10 +234,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -267,9 +279,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -302,26 +314,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -354,26 +349,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -549,17 +527,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -591,7 +569,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
@@ -623,7 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -655,7 +633,7 @@
         <v>-95.371262999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -687,7 +665,7 @@
         <v>-95.371262999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -719,7 +697,7 @@
         <v>-95.371262999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -751,7 +729,7 @@
         <v>-95.371262999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -783,11 +761,11 @@
         <v>-95.371262999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C8" t="s">
@@ -815,7 +793,7 @@
         <v>-95.371262999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -847,7 +825,7 @@
         <v>-106.461641</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -879,7 +857,7 @@
         <v>-106.461641</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -911,7 +889,7 @@
         <v>-106.461641</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -943,7 +921,7 @@
         <v>-106.461641</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -978,7 +956,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1013,7 +991,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1045,7 +1023,7 @@
         <v>-101.86396999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1077,7 +1055,7 @@
         <v>-98.700410000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1109,7 +1087,7 @@
         <v>-95.534903</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1141,7 +1119,7 @@
         <v>-94.976112000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1173,7 +1151,7 @@
         <v>-94.976112000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>

</xml_diff>